<commit_message>
Second shot at filling employees
</commit_message>
<xml_diff>
--- a/SnelStartEmployeeExport0001.xlsx
+++ b/SnelStartEmployeeExport0001.xlsx
@@ -38,9 +38,6 @@
     <t>creditcard00018</t>
   </si>
   <si>
-    <t>NaamWerknemer1</t>
-  </si>
-  <si>
     <t>AdresWerknemer1</t>
   </si>
   <si>
@@ -53,6 +50,9 @@
     <t>Adres3Werknemer1</t>
   </si>
   <si>
+    <t>Adres4Werknemer1</t>
+  </si>
+  <si>
     <t>TelefoonWerknemer1</t>
   </si>
   <si>
@@ -77,9 +77,6 @@
     <t>creditcard0002</t>
   </si>
   <si>
-    <t>NaamWerknemer2</t>
-  </si>
-  <si>
     <t>AdresWerknemer2</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>Adres3Werknemer2</t>
+  </si>
+  <si>
+    <t>Adres4Werknemer2</t>
   </si>
   <si>
     <t>TelefoonWerknemer2</t>
@@ -108,7 +108,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -129,11 +129,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -178,16 +173,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -211,15 +202,13 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q2" activeCellId="0" sqref="Q2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="17" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="21.3928571428571"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="30.8418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="20" min="1" style="0" width="11.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -259,10 +248,10 @@
       <c r="L1" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="0" t="s">
         <v>8</v>
       </c>
       <c r="O1" s="0" t="s">
@@ -321,13 +310,13 @@
       <c r="L2" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="0" t="s">
         <v>22</v>
       </c>
       <c r="P2" s="0" t="s">
@@ -336,7 +325,7 @@
       <c r="Q2" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="1" t="s">
         <v>25</v>
       </c>
       <c r="S2" s="0" t="s">

</xml_diff>